<commit_message>
Correções no plano de aulas do site.
</commit_message>
<xml_diff>
--- a/plano-de-aulas-t2.xlsx
+++ b/plano-de-aulas-t2.xlsx
@@ -529,8 +529,8 @@
   </sheetPr>
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1881,6 +1881,12 @@
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1002" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Aulas 05 e 06
</commit_message>
<xml_diff>
--- a/plano-de-aulas-t2.xlsx
+++ b/plano-de-aulas-t2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Passagem de argumentos por referência e valor; Recursos de C++.</t>
   </si>
   <si>
+    <t xml:space="preserve">Utilização de ferramentas de profiling para identificar pontos quentes em um programa.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estratégias para solução de problemas dificeis</t>
   </si>
   <si>
@@ -80,46 +83,46 @@
     <t xml:space="preserve">Utilização de sorteios aleatórios em algoritmos de busca local e heurísticas.</t>
   </si>
   <si>
+    <t xml:space="preserve">Buscando uma solução globalmente ótima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busca global vs Busca local; Enumeração exaustiva e sua classe de problemas computacionais; Backtracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de algoritmo de enumeração exaustiva em C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gap de otimalidade; Simetrias; Comunicação de resultados de desempenho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de algoritmo de enumeração exaustiva em C++; Comparação entre soluções ótimas e sub-ótimas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quando uma otimização vale a pena? Qual método é o mais eficaz em resolver um problema?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análise de resultados de execução</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comparação entre soluções ótimas e sub-ótimas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acelerando a busca local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimando a qualidade de uma solução parcial; Medindo a efetividade de uma estimativa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de branch-and-bound; Comparação de dois bounds diferentes para o mesmo problema. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indo além: best-first search, simetrias, competição de desempenho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva sobre melhorias possíveis além do branch-and-bound.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aula estúdio para projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscando uma solução globalmente ótima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Busca global vs Busca local; Enumeração exaustiva e sua classe de problemas computacionais; Backtracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de algoritmo de enumeração exaustiva em C++</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gap de otimalidade; Simetrias; Comunicação de resultados de desempenho.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de algoritmo de enumeração exaustiva em C++; Comparação entre soluções ótimas e sub-ótimas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quando uma otimização vale a pena? Qual método é o mais eficaz em resolver um problema?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análise de resultados de execução</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comparação entre soluções ótimas e sub-ótimas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acelerando a busca local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimando a qualidade de uma solução parcial; Medindo a efetividade de uma estimativa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de branch-and-bound; Comparação de dois bounds diferentes para o mesmo problema. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indo além: best-first search, simetrias, competição de desempenho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula expositiva sobre melhorias possíveis além do branch-and-bound.</t>
   </si>
   <si>
     <t xml:space="preserve">Feriado</t>
@@ -244,7 +247,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,13 +257,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFCD4D1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
         <bgColor rgb="FFFCD3C1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD3C1"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFCD4D1"/>
       </patternFill>
     </fill>
     <fill>
@@ -270,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -286,34 +295,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -325,6 +306,13 @@
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -353,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -382,51 +370,43 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,19 +414,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,7 +459,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -529,8 +509,8 @@
   </sheetPr>
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34:E48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -662,22 +642,22 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <f aca="false">A2+7</f>
         <v>44258</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -702,22 +682,22 @@
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <f aca="false">A3+7</f>
         <v>44260</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -742,22 +722,22 @@
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <f aca="false">A4+7</f>
         <v>44265</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -788,15 +768,15 @@
         <v>44267</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="8"/>
@@ -827,16 +807,16 @@
         <f aca="false">A6+7</f>
         <v>44272</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="8"/>
@@ -867,16 +847,16 @@
         <f aca="false">A7+7</f>
         <v>44274</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="8"/>
@@ -902,21 +882,21 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="87.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <f aca="false">A8+7</f>
         <v>44279</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="8"/>
@@ -947,16 +927,16 @@
         <f aca="false">A9+7</f>
         <v>44281</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="8"/>
@@ -987,17 +967,17 @@
         <f aca="false">A10+7</f>
         <v>44286</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>19</v>
+      <c r="E12" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -1027,17 +1007,17 @@
         <f aca="false">A11+7</f>
         <v>44288</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>33</v>
+      <c r="B13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
@@ -1067,17 +1047,17 @@
         <f aca="false">A12+7</f>
         <v>44293</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>34</v>
+      <c r="B14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
@@ -1107,17 +1087,17 @@
         <f aca="false">A13+7</f>
         <v>44295</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>34</v>
+      <c r="B15" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
@@ -1147,17 +1127,17 @@
         <f aca="false">A14+7</f>
         <v>44300</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>34</v>
+      <c r="B16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
@@ -1187,17 +1167,17 @@
         <f aca="false">A15+7</f>
         <v>44302</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>37</v>
+      <c r="E17" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
@@ -1255,17 +1235,17 @@
         <f aca="false">A17+7</f>
         <v>44309</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="B19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>39</v>
+      <c r="E19" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
@@ -1295,17 +1275,17 @@
         <f aca="false">A18+7</f>
         <v>44314</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="B20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>41</v>
+      <c r="E20" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
@@ -1335,17 +1315,17 @@
         <f aca="false">A19+7</f>
         <v>44316</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="D21" s="12" t="s">
         <v>44</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9"/>
@@ -1375,17 +1355,17 @@
         <f aca="false">A20+7</f>
         <v>44321</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>19</v>
+      <c r="B22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
@@ -1415,17 +1395,17 @@
         <f aca="false">A21+7</f>
         <v>44323</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>19</v>
+      <c r="B23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
@@ -1455,17 +1435,17 @@
         <f aca="false">A22+7</f>
         <v>44328</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="12" t="s">
         <v>48</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
@@ -1495,17 +1475,17 @@
         <f aca="false">A23+7</f>
         <v>44330</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="D25" s="12" t="s">
         <v>48</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
@@ -1535,17 +1515,17 @@
         <f aca="false">A24+7</f>
         <v>44335</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="B26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>50</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
@@ -1575,17 +1555,17 @@
         <f aca="false">A25+7</f>
         <v>44337</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="B27" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>52</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
@@ -1615,17 +1595,17 @@
         <f aca="false">A26+7</f>
         <v>44342</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="B28" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>54</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
@@ -1655,17 +1635,17 @@
         <f aca="false">A27+7</f>
         <v>44344</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>55</v>
+      <c r="B29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
@@ -1695,17 +1675,17 @@
         <f aca="false">A28+7</f>
         <v>44349</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>19</v>
+      <c r="B30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
@@ -1735,17 +1715,17 @@
         <f aca="false">A29+7</f>
         <v>44351</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>33</v>
+      <c r="B31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="10"/>
@@ -1775,17 +1755,17 @@
         <f aca="false">A30+7</f>
         <v>44356</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>34</v>
+      <c r="B32" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="10"/>
@@ -1815,17 +1795,17 @@
         <f aca="false">A31+7</f>
         <v>44358</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>34</v>
+      <c r="B33" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="10"/>
@@ -1851,27 +1831,27 @@
       <c r="AA33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="51.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
-      <c r="X34" s="23"/>
-      <c r="Y34" s="23"/>
-      <c r="Z34" s="23"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
+      <c r="Z34" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>